<commit_message>
updated test case id to 7 from 9
</commit_message>
<xml_diff>
--- a/OrderData.xlsx
+++ b/OrderData.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -349,7 +350,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -364,7 +365,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>